<commit_message>
- Sprint 1 Update
</commit_message>
<xml_diff>
--- a/excel-app/$Product Backlog.xlsx
+++ b/excel-app/$Product Backlog.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlolg" sheetId="1" r:id="rId1"/>
     <sheet name="Ceremonies" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
   <si>
     <t>Sprint Planning</t>
   </si>
@@ -42,83 +42,119 @@
     <t>Demo and obtain feedback</t>
   </si>
   <si>
-    <t>Establish and Document all practices and tools (Case Study) (Very simple, maybe just a descriptioin and a url. (Adrienne write a blog?)
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>IOGR 1995: http://laws-lois.justice.gc.ca/eng/regulations/SOR-94-753/index.html</t>
+  </si>
+  <si>
+    <t>Sask Oil</t>
+  </si>
+  <si>
+    <t>GOOR</t>
+  </si>
+  <si>
+    <t>Calculations</t>
+  </si>
+  <si>
+    <t>Work Sheets</t>
+  </si>
+  <si>
+    <t>Sask Gas</t>
+  </si>
+  <si>
+    <t>Alta Oil</t>
+  </si>
+  <si>
+    <t>Alta Gas</t>
+  </si>
+  <si>
+    <t>Create new project???</t>
+  </si>
+  <si>
+    <t>Create Data Access Strategy</t>
+  </si>
+  <si>
+    <t>Refreash</t>
+  </si>
+  <si>
+    <t>Create TDD Strategy  (Coverage, No Code without a test)</t>
+  </si>
+  <si>
+    <t>Create Data Utilities (Copy from excel to sqlite, sqlite to excel, test strategy)</t>
+  </si>
+  <si>
+    <t>Start implementing component by component</t>
+  </si>
+  <si>
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>Royalty Master</t>
+  </si>
+  <si>
+    <t>Well</t>
+  </si>
+  <si>
+    <t>By Payer</t>
+  </si>
+  <si>
+    <t>By Area</t>
+  </si>
+  <si>
+    <t>By Lease</t>
+  </si>
+  <si>
+    <t>By …</t>
+  </si>
+  <si>
+    <t>Create a reporting strategy</t>
+  </si>
+  <si>
+    <t>Help System</t>
+  </si>
+  <si>
+    <t>Establish and Document all practices and tools (Case Study) (Very simple, maybe just a descriptioin and a url. (Adrienne write a blog?) Best Practices
 - Scrum, Python, GIT, TDD, Flask,  sqlite, sql…</t>
   </si>
   <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>IOGR 1995: http://laws-lois.justice.gc.ca/eng/regulations/SOR-94-753/index.html</t>
-  </si>
-  <si>
-    <t>Sask Oil</t>
-  </si>
-  <si>
-    <t>GOOR</t>
-  </si>
-  <si>
-    <t>Calculations</t>
-  </si>
-  <si>
-    <t>Work Sheets</t>
-  </si>
-  <si>
-    <t>Sask Gas</t>
-  </si>
-  <si>
-    <t>Alta Oil</t>
-  </si>
-  <si>
-    <t>Alta Gas</t>
-  </si>
-  <si>
-    <t>Create new project???</t>
-  </si>
-  <si>
-    <t>Create Data Access Strategy</t>
-  </si>
-  <si>
-    <t>Refreash</t>
-  </si>
-  <si>
-    <t>Create TDD Strategy  (Coverage, No Code without a test)</t>
-  </si>
-  <si>
-    <t>Create Data Utilities (Copy from excel to sqlite, sqlite to excel, test strategy)</t>
-  </si>
-  <si>
-    <t>Start implementing component by component</t>
-  </si>
-  <si>
-    <t>CRUD</t>
-  </si>
-  <si>
-    <t>Reports</t>
-  </si>
-  <si>
-    <t>Royalty Master</t>
-  </si>
-  <si>
-    <t>Well</t>
-  </si>
-  <si>
-    <t>By Payer</t>
-  </si>
-  <si>
-    <t>By Area</t>
-  </si>
-  <si>
-    <t>By Lease</t>
-  </si>
-  <si>
-    <t>By …</t>
-  </si>
-  <si>
-    <t>Create a reporting strategy</t>
+    <t>Validate Worksheet and Calc for SaskCrown Oil</t>
+  </si>
+  <si>
+    <t>Add worksheet to GUI</t>
+  </si>
+  <si>
+    <t>Hours</t>
+  </si>
+  <si>
+    <t>Adrienne Learn python test</t>
+  </si>
+  <si>
+    <t>Get System running on Adrienne's machine</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Review and Learn Existing Calcs</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
   </si>
 </sst>
 </file>
@@ -126,7 +162,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -199,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -508,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,10 +569,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="3">
         <v>42388</v>
@@ -561,157 +597,182 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
+    <row r="14" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>14</v>
+      <c r="A18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>17</v>
+      <c r="A23" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>15</v>
+      <c r="A26" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>17</v>
+      <c r="A31" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>25</v>
+      <c r="A34" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -773,12 +834,131 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="54.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- updated product backlog
</commit_message>
<xml_diff>
--- a/excel-app/$Product Backlog.xlsx
+++ b/excel-app/$Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>Sprint Planning</t>
   </si>
@@ -148,13 +148,49 @@
     <t>A</t>
   </si>
   <si>
-    <t>Review and Learn Existing Calcs</t>
-  </si>
-  <si>
     <t>Tue</t>
   </si>
   <si>
     <t>Wed</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>Get TDD running in Adrienne's machine</t>
+  </si>
+  <si>
+    <t>K&amp;A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review and Learn Existing Calcs </t>
+  </si>
+  <si>
+    <t>Setup new project and new dirctory structure</t>
+  </si>
+  <si>
+    <t>Create a model module with tests and convensions (Where do our test go, nameing convension)</t>
+  </si>
+  <si>
+    <t>Implement Missing IOGR1995 Supplementary Royalty with tests</t>
+  </si>
+  <si>
+    <t>Write Tests and restructure calcSaskOilProvCrown</t>
+  </si>
+  <si>
+    <t>Write DB Load utilities for testing</t>
+  </si>
+  <si>
+    <t>Adrienne - Test Drivin Development, Python code</t>
+  </si>
+  <si>
+    <t>Konstantin - sqlite, calcs</t>
+  </si>
+  <si>
+    <t>Larry - Utilities help</t>
   </si>
 </sst>
 </file>
@@ -834,131 +870,210 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D14"/>
+  <dimension ref="A2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" style="2" customWidth="1"/>
+    <col min="2" max="3" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>38</v>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
-      <c r="C10">
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B25" t="s">
         <v>40</v>
       </c>
-      <c r="C13">
+      <c r="D25">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B26" t="s">
         <v>41</v>
       </c>
-      <c r="C14">
+      <c r="D26">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Updates as a result of day working as a team
</commit_message>
<xml_diff>
--- a/excel-app/$Product Backlog.xlsx
+++ b/excel-app/$Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>Sprint Planning</t>
   </si>
@@ -148,9 +148,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>Tue</t>
-  </si>
-  <si>
     <t>Wed</t>
   </si>
   <si>
@@ -191,6 +188,36 @@
   </si>
   <si>
     <t>Larry - Utilities help</t>
+  </si>
+  <si>
+    <t>Create Data Access Strategy Step 1 example</t>
+  </si>
+  <si>
+    <t>Dane</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>Refactor DB Load with test</t>
+  </si>
+  <si>
+    <t>Write the our version of orm</t>
+  </si>
+  <si>
+    <t>Read organization of tests</t>
+  </si>
+  <si>
+    <t>Complete tests IORG1995</t>
+  </si>
+  <si>
+    <t>Complete tests for Sask CrownRoyalty Rate</t>
+  </si>
+  <si>
+    <t>Brake out Used Royalty Rate</t>
+  </si>
+  <si>
+    <t>Finish IOGR1995</t>
   </si>
 </sst>
 </file>
@@ -870,10 +897,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E26"/>
+  <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,191 +911,271 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
       <c r="E3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17">
-        <v>3</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20">
-        <v>7</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21">
-        <v>3</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>45</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
       </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
       <c r="D25">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
         <v>41</v>
       </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
       <c r="D26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Update Product Backlog
</commit_message>
<xml_diff>
--- a/excel-app/$Product Backlog.xlsx
+++ b/excel-app/$Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
   <si>
     <t>Sprint Planning</t>
   </si>
@@ -218,6 +218,45 @@
   </si>
   <si>
     <t>Finish IOGR1995</t>
+  </si>
+  <si>
+    <t>Moving to the new World</t>
+  </si>
+  <si>
+    <t>- sqlite - complete base functions to replace excel sheets</t>
+  </si>
+  <si>
+    <t>- Update naming convensions</t>
+  </si>
+  <si>
+    <t>- Move to new directory structure</t>
+  </si>
+  <si>
+    <t>Incorporate Prod Date in App</t>
+  </si>
+  <si>
+    <t>Incorporate Effective Date</t>
+  </si>
+  <si>
+    <t>Add WIO concept</t>
+  </si>
+  <si>
+    <t>Update GUI to look nice</t>
+  </si>
+  <si>
+    <t>Update GUI to actually update</t>
+  </si>
+  <si>
+    <t>More Calculations</t>
+  </si>
+  <si>
+    <t>More Reports</t>
+  </si>
+  <si>
+    <t>More Browses</t>
+  </si>
+  <si>
+    <t>Mapping Stuff (Just show a little)</t>
   </si>
 </sst>
 </file>
@@ -289,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -303,6 +342,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,10 +939,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E34"/>
+  <dimension ref="A2:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,258 +966,323 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
+      <c r="A6" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7">
-        <v>14</v>
+      <c r="A7" s="5" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
+      <c r="A8" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11">
-        <v>5</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
         <v>40</v>
       </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
       <c r="D24">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
       </c>
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
       <c r="D25">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D26">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s">
         <v>42</v>
       </c>
-      <c r="C28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28">
-        <v>7</v>
+      <c r="D27">
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
         <v>42</v>
-      </c>
-      <c r="C31" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B50" t="s">
         <v>41</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C50" t="s">
         <v>58</v>
       </c>
-      <c r="D34">
+      <c r="D50">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
a few edits to worksheet and updated product backlog
</commit_message>
<xml_diff>
--- a/excel-app/$Product Backlog.xlsx
+++ b/excel-app/$Product Backlog.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24526"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="25600" yWindow="0" windowWidth="25600" windowHeight="20480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlolg" sheetId="1" r:id="rId1"/>
     <sheet name="Ceremonies" sheetId="2" r:id="rId2"/>
     <sheet name="Sprint1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="123">
   <si>
     <t>Sprint Planning</t>
   </si>
@@ -181,9 +187,6 @@
     <t>Write DB Load utilities for testing</t>
   </si>
   <si>
-    <t>Adrienne - Test Drivin Development, Python code</t>
-  </si>
-  <si>
     <t>Konstantin - sqlite, calcs</t>
   </si>
   <si>
@@ -305,16 +308,101 @@
   </si>
   <si>
     <t>- Konstantin</t>
+  </si>
+  <si>
+    <t>Adrienne - Test Driven Development, Python code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Konstantin </t>
+  </si>
+  <si>
+    <t>-Review existing code to follow the convention</t>
+  </si>
+  <si>
+    <t>Adrienne</t>
+  </si>
+  <si>
+    <t>-Review existing code (calc and worksheet) to follow the convention</t>
+  </si>
+  <si>
+    <t>Larry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Larry go over all utility functions </t>
+  </si>
+  <si>
+    <t>-Remove excel dependencies from new structure</t>
+  </si>
+  <si>
+    <t>-Move data utility to new structure</t>
+  </si>
+  <si>
+    <t>-Move excel load to new structure</t>
+  </si>
+  <si>
+    <t>-Move obfuscator to the new structure</t>
+  </si>
+  <si>
+    <t>-Rearrange menu to have infrastructure</t>
+  </si>
+  <si>
+    <t>-Basic security profiles</t>
+  </si>
+  <si>
+    <t>-Get running for all calculation types</t>
+  </si>
+  <si>
+    <t>-Take first shot at prodMonth</t>
+  </si>
+  <si>
+    <t>Lorraine</t>
+  </si>
+  <si>
+    <t>-Work with Larry to review the obf word techniques</t>
+  </si>
+  <si>
+    <t>-Review worksheet from user perspective</t>
+  </si>
+  <si>
+    <t>-Provide liaison between business and development</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Load RM for data </t>
+  </si>
+  <si>
+    <t>-Load well RM link</t>
+  </si>
+  <si>
+    <t>Important</t>
+  </si>
+  <si>
+    <t>-Make calc and worksheet accessible to user from browser</t>
+  </si>
+  <si>
+    <t>-Come up with first cut of format of browse of external data</t>
+  </si>
+  <si>
+    <t>-Program first cut of browse of external data</t>
+  </si>
+  <si>
+    <t>-Program worksheet format changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Everyone working in new structure </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +423,36 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -361,22 +479,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -402,8 +529,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="10">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -462,7 +603,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -497,7 +638,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -708,25 +849,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="74.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -752,194 +893,199 @@
         <v>42416</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="47.25" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1">
       <c r="A29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1">
       <c r="A32" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1">
       <c r="A39" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1">
       <c r="A44" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -951,13 +1097,13 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="2" width="72.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="2" max="2" width="72.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -965,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -973,7 +1119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -981,7 +1127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -991,6 +1137,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -998,214 +1149,244 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="54.5703125" style="2" customWidth="1"/>
-    <col min="2" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="54.5" style="2" customWidth="1"/>
+    <col min="2" max="3" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="6">
         <v>42445</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="E3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="8" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="8" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" s="8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="8"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="8"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+    <row r="26" spans="1:1">
+      <c r="A26" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="8"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:1">
+      <c r="A30" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+    <row r="31" spans="1:1">
+      <c r="A31" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="32" spans="1:1">
+      <c r="A32" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="34" spans="1:4">
+      <c r="A34" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:4">
+      <c r="A40" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:4">
+      <c r="A41" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
@@ -1214,9 +1395,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B45" t="s">
         <v>42</v>
@@ -1225,9 +1406,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
         <v>40</v>
@@ -1236,9 +1417,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
         <v>40</v>
@@ -1247,9 +1428,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B48" t="s">
         <v>40</v>
@@ -1258,9 +1439,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
         <v>42</v>
@@ -1269,9 +1450,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
         <v>42</v>
@@ -1280,7 +1461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>35</v>
       </c>
@@ -1291,7 +1472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>49</v>
       </c>
@@ -1299,7 +1480,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="28">
       <c r="A54" s="2" t="s">
         <v>50</v>
       </c>
@@ -1307,7 +1488,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4">
       <c r="A55" s="2" t="s">
         <v>51</v>
       </c>
@@ -1315,7 +1496,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>52</v>
       </c>
@@ -1323,27 +1504,27 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4">
       <c r="A59" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+    <row r="61" spans="1:4">
+      <c r="A61" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4">
       <c r="A63" s="2" t="s">
         <v>6</v>
       </c>
@@ -1357,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>36</v>
       </c>
@@ -1371,7 +1552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>7</v>
       </c>
@@ -1385,7 +1566,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4">
       <c r="A67" s="2" t="s">
         <v>38</v>
       </c>
@@ -1399,7 +1580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
         <v>39</v>
       </c>
@@ -1413,7 +1594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
         <v>46</v>
       </c>
@@ -1421,7 +1602,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
         <v>48</v>
       </c>
@@ -1432,7 +1613,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
         <v>21</v>
       </c>
@@ -1446,15 +1627,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B73" t="s">
         <v>41</v>
       </c>
       <c r="C73" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D73">
         <v>10</v>
@@ -1462,6 +1643,246 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="6">
+        <v>42461</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" s="11"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="B25" s="10"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>110</v>
+      </c>
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="10" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>